<commit_message>
actualizacion de cierre cambio proyecto
</commit_message>
<xml_diff>
--- a/Proyectos/ControlDeGastos/07. Control de Cambios/ControldeGastos-SolicitudCambio.xlsx
+++ b/Proyectos/ControlDeGastos/07. Control de Cambios/ControldeGastos-SolicitudCambio.xlsx
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Datos Generales</t>
   </si>
@@ -130,7 +130,7 @@
     <t>Estado del Cambio</t>
   </si>
   <si>
-    <t>Abierto</t>
+    <t>Cerrado</t>
   </si>
   <si>
     <t>Identificación del Cambio</t>
@@ -217,10 +217,16 @@
     <t>Revisor:</t>
   </si>
   <si>
+    <t>Jovanny Zepeda</t>
+  </si>
+  <si>
     <t>Fecha de Resolución:</t>
   </si>
   <si>
     <t>Resultado:</t>
+  </si>
+  <si>
+    <t>Aprobado</t>
   </si>
   <si>
     <t>Estado General del Cambio:</t>
@@ -254,9 +260,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -364,7 +371,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -401,6 +408,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -409,15 +420,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -498,15 +509,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1013760</xdr:colOff>
+      <xdr:colOff>1040760</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>537840</xdr:colOff>
+      <xdr:colOff>564480</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>139320</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -519,8 +530,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8507880" y="19080"/>
-          <a:ext cx="1869120" cy="1910880"/>
+          <a:off x="8534880" y="10080"/>
+          <a:ext cx="1868760" cy="1910520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -530,51 +541,6 @@
         </a:ln>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>388440</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>190440</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="27000" y="0"/>
-          <a:ext cx="11242080" cy="6769440"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="ffffff"/>
-        </a:solidFill>
-        <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -587,8 +553,8 @@
   </sheetPr>
   <dimension ref="B1:F65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -730,100 +696,112 @@
       <c r="D16" s="5" t="n">
         <v>42475</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="9" t="n">
+        <v>42494</v>
+      </c>
       <c r="F16" s="8" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="10" t="n">
         <f aca="false">SUM(F16:F16)</f>
         <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="10"/>
+      <c r="C19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="10" t="n">
         <f aca="false">75*15</f>
         <v>1125</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="10" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="10" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="12" t="n">
+        <v>42494</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="11" t="n">
+      <c r="C24" s="13" t="n">
         <v>42476</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="11" t="n">
+      <c r="C25" s="13" t="n">
         <v>42476</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
     </row>
     <row r="27" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="12" t="n">
+        <v>42494</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="9"/>
+      <c r="C28" s="10" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="9"/>
+      <c r="B29" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="12" t="n">
+        <v>42494</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="13"/>
+      <c r="B30" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -899,39 +877,39 @@
         <v>26</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>